<commit_message>
Cập nhật danh sách cổ đông mẫu và danh sách ủy quyền mẫu.
</commit_message>
<xml_diff>
--- a/Danh_sach_co_dong_mau.xlsx
+++ b/Danh_sach_co_dong_mau.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\job\bedhcd\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BBE7A2-6703-4D47-95D8-9789C0579370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3615" yWindow="2430" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3620" yWindow="2430" windowWidth="21600" windowHeight="11390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -133,7 +127,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -484,22 +478,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -537,7 +532,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -575,7 +570,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -610,7 +605,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
feat: Thêm chức năng nhập dữ liệu cổ đông và ủy quyền từ tệp Excel, cùng với cấu hình ứng dụng ban đầu.
</commit_message>
<xml_diff>
--- a/Danh_sach_co_dong_mau.xlsx
+++ b/Danh_sach_co_dong_mau.xlsx
@@ -1,20 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Private\project_dhcd\bedhcd\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495D54BB-71C4-4DA9-A7BD-A13096E196AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3620" yWindow="2430" windowWidth="21600" windowHeight="11390"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <extLst>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>STT</t>
   </si>
@@ -122,12 +133,15 @@
   </si>
   <si>
     <t>pass123</t>
+  </si>
+  <si>
+    <t>SH004</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -478,23 +492,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.81640625" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -532,7 +546,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -570,7 +584,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -605,7 +619,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -641,6 +655,35 @@
       </c>
       <c r="L4" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5">
+        <v>200</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="3">
+        <v>42040</v>
       </c>
     </row>
   </sheetData>

</xml_diff>